<commit_message>
added security against crashes due to not finding elements
</commit_message>
<xml_diff>
--- a/supporting_files/contacts.xlsx
+++ b/supporting_files/contacts.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\GitHub\MissionHubHelper\supporting_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9FC64D-C7CE-4EC0-9876-EF78C98FFF02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="19390" windowHeight="10390"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
-  <si>
-    <t>Malet??</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>First Name</t>
   </si>
@@ -39,34 +36,10 @@
     <t>Full Name</t>
   </si>
   <si>
-    <t>Andrew Lee</t>
-  </si>
-  <si>
-    <t>Kevin Horn</t>
-  </si>
-  <si>
     <t>Phone Number</t>
   </si>
   <si>
     <t>Phone number formatted</t>
-  </si>
-  <si>
-    <t>Beth Ann Emery</t>
-  </si>
-  <si>
-    <t>Connor</t>
-  </si>
-  <si>
-    <t>Hey</t>
-  </si>
-  <si>
-    <t>This</t>
-  </si>
-  <si>
-    <t>Is</t>
-  </si>
-  <si>
-    <t>Helpful</t>
   </si>
   <si>
     <t>Gender</t>
@@ -183,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -815,485 +788,458 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.3671875" customWidth="1"/>
+    <col min="2" max="2" width="18.5234375" style="3" customWidth="1"/>
     <col min="3" max="3" width="12" style="18" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="10.89453125" customWidth="1"/>
+    <col min="5" max="5" width="11.5234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.15625" customWidth="1"/>
+    <col min="7" max="7" width="10.62890625" customWidth="1"/>
+    <col min="8" max="8" width="11.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="18"/>
+      <c r="B2" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="D2" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="18"/>
+      <c r="B3" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="18"/>
+      <c r="B4" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="18"/>
+      <c r="B5" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="31" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="22"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>23</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="19"/>
     </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="18" t="s">
-        <v>9</v>
-      </c>
+    <row r="6" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="18"/>
       <c r="B6" s="31" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C6" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>24</v>
-      </c>
       <c r="E6" s="31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="18"/>
       <c r="B7" s="31" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="18"/>
       <c r="B8" s="31" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="18"/>
       <c r="B9" s="31" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="18" t="s">
-        <v>10</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="18"/>
       <c r="B10" s="31" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="19"/>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="18" t="s">
-        <v>11</v>
-      </c>
+    <row r="11" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A11" s="18"/>
       <c r="B11" s="31" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="18" t="s">
-        <v>12</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A12" s="18"/>
       <c r="B12" s="31" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F12" s="19"/>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="18" t="s">
-        <v>13</v>
-      </c>
+    <row r="13" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A13" s="18"/>
       <c r="B13" s="31" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="18"/>
       <c r="B14" s="24"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="18"/>
       <c r="B15" s="24"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="18"/>
       <c r="B16" s="24"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="19"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="18"/>
       <c r="B17" s="24"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="18"/>
       <c r="B18" s="24"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="19"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="18"/>
       <c r="B19" s="24"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="18"/>
       <c r="B20" s="24"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="18"/>
       <c r="B21" s="24"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="16"/>
       <c r="D22" s="5"/>
       <c r="E22" s="7"/>
       <c r="F22" s="27"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="17"/>
       <c r="D23" s="4"/>
       <c r="E23" s="6"/>
       <c r="F23" s="28"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="16"/>
       <c r="D24" s="5"/>
       <c r="E24" s="7"/>
       <c r="F24" s="29"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="25"/>
       <c r="D25" s="11"/>
       <c r="E25" s="12"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="17"/>
       <c r="D26" s="4"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="16"/>
       <c r="D27" s="13"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="17"/>
       <c r="D28" s="4"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="16"/>
       <c r="D29" s="13"/>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="17"/>
       <c r="D30" s="4"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="16"/>
       <c r="D31" s="13"/>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="17"/>
       <c r="D32" s="4"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="16"/>
       <c r="D33" s="13"/>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="17"/>
       <c r="D34" s="4"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="26"/>
       <c r="D35" s="14"/>
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="26"/>
       <c r="D36" s="14"/>
       <c r="E36" s="15"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="24"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="24"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="24"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="24"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="24"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="2"/>
       <c r="D42" s="1"/>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="2"/>
       <c r="D43" s="1"/>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E44" s="9"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E45" s="9"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E46" s="9"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E47" s="9"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E48" s="9"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E49" s="9"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E50" s="9"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E52" s="9"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E58" s="9"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E60" s="9"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E61" s="9"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E62" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{F7C9EE02-42E1-4005-9D12-6889AFFD525C}">
-      <x15:webExtensions xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x15:webExtension appRef="{2105D1D0-6DFA-4A12-BB12-F853D08C7FC0}">
-          <xm:f>Sheet1!$H$43</xm:f>
-        </x15:webExtension>
-      </x15:webExtensions>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lots of problems fixed
A few bugs found with a 'dirtier' dataset fixed
</commit_message>
<xml_diff>
--- a/supporting_files/contacts.xlsx
+++ b/supporting_files/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\GitHub\MissionHubHelper\supporting_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754ABAFC-1286-4A2B-A6FD-B1AC89368768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6E48B3-B750-4952-8DFC-58EB2EC5223A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>First Name</t>
   </si>
@@ -46,13 +46,157 @@
   </si>
   <si>
     <t>Gender formatted</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Kalli</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Stephanie</t>
+  </si>
+  <si>
+    <t>Laynez</t>
+  </si>
+  <si>
+    <t>Joyce</t>
+  </si>
+  <si>
+    <t>He</t>
+  </si>
+  <si>
+    <t>Lauren</t>
+  </si>
+  <si>
+    <t>Oevermann</t>
+  </si>
+  <si>
+    <t>Faulkner</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Harper</t>
+  </si>
+  <si>
+    <t>Caitie</t>
+  </si>
+  <si>
+    <t>Huff</t>
+  </si>
+  <si>
+    <t>Hailey</t>
+  </si>
+  <si>
+    <t>Giles</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>Whalen</t>
+  </si>
+  <si>
+    <t>Rylie</t>
+  </si>
+  <si>
+    <t>Riddle</t>
+  </si>
+  <si>
+    <t>Samantha</t>
+  </si>
+  <si>
+    <t>Jeanelle</t>
+  </si>
+  <si>
+    <t>Oloyo</t>
+  </si>
+  <si>
+    <t>Paula</t>
+  </si>
+  <si>
+    <t>Diaz</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Pietersz</t>
+  </si>
+  <si>
+    <t>Stein</t>
+  </si>
+  <si>
+    <t>Amari</t>
+  </si>
+  <si>
+    <t>Mapp</t>
+  </si>
+  <si>
+    <t>Leul</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Aguilar</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>Garza</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>aalaysiah</t>
+  </si>
+  <si>
+    <t>morrison</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Mahavier</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Prestwood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lulia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elsy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blanco </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,19 +211,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +252,12 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -132,26 +288,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -159,6 +307,26 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,274 +641,624 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.3671875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="18.5234375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.89453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.5234375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.15625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="10.62890625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="11.47265625" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="8.83984375" style="7"/>
+    <col min="1" max="1" width="15.3671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.5234375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.89453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.15625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="10.62890625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="11.47265625" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="8.83984375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13">
+        <v>5129442224</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13">
+        <v>5129875421</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13">
+        <v>2542957260</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13">
+        <v>2102436579</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13">
+        <v>8177264771</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13">
+        <v>6828082508</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="15">
+        <v>8066761132</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13">
+        <v>4436190267</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13">
+        <v>2107183423</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13">
+        <v>9568026229</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13">
+        <v>8066789201</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="15">
+        <v>8324210986</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="2"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13">
+        <v>2144253105</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="2"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13">
+        <v>2147188294</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="2"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="2"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="2"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="2"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="2"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="2"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="2"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="2"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" s="2"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B25" s="2"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="2"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="2"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" s="2"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" s="2"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="2"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31" s="2"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="2"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="2"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34" s="2"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B35" s="2"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36" s="2"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B37" s="2"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B38" s="2"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B39" s="2"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B40" s="2"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B41" s="2"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="2"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43" s="2"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13">
+        <v>2109989692</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13">
+        <v>2067957492</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13">
+        <v>5126355765</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13">
+        <v>2107925272</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13">
+        <v>8328363654</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="13"/>
+      <c r="B21" s="15">
+        <v>4696051471</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="13"/>
+      <c r="B22" s="15">
+        <v>2815434485</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="13"/>
+      <c r="B23" s="15">
+        <v>7132778108</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13">
+        <v>3619468307</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="10"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="10"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="10"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="10"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="10"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="10"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="10"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="10"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="10"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="10"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="10"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" s="9"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" s="9"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" s="9"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" s="9"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="9"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" s="9"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" s="9"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" s="9"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" s="9"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" s="9"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="9"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" s="9"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" s="9"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" s="9"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" s="9"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" s="9"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" s="9"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" s="9"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" s="9"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" s="9"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56" s="9"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" s="9"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58" s="9"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59" s="9"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60" s="9"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" selectLockedCells="1" sort="0"/>
+  <sheetProtection formatCells="0" selectLockedCells="1" sort="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adds year tag and notes
</commit_message>
<xml_diff>
--- a/supporting_files/contacts.xlsx
+++ b/supporting_files/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\GitHub\MissionHubHelper\supporting_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339E099D-F07F-4102-950C-685820EB12D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E186EF4-4D89-47D1-854F-D492D2C5E355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="108">
   <si>
     <t>First Name</t>
   </si>
@@ -316,6 +316,39 @@
   </si>
   <si>
     <t xml:space="preserve">Trevino </t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Year formatted</t>
+  </si>
+  <si>
+    <t>fresh</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>fre</t>
+  </si>
+  <si>
+    <t>soph</t>
+  </si>
+  <si>
+    <t>senior</t>
+  </si>
+  <si>
+    <t>junior</t>
+  </si>
+  <si>
+    <t>yo</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -423,9 +456,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -441,6 +471,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,27 +786,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="15.3671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="18.5234375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.89453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.15625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="10.62890625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="11.47265625" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="8.83984375" style="5"/>
+    <col min="3" max="5" width="12" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.89453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.5234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.15625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.62890625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="11.47265625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.83984375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -786,768 +817,912 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12">
+      <c r="J1" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11">
         <v>5129442224</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="11">
+        <v>2024</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11">
         <v>5129875421</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11">
         <v>2542957260</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11">
         <v>2102436579</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11">
         <v>8177264771</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11">
         <v>6828082508</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11">
         <v>4436190267</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11">
         <v>2107183423</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11">
         <v>9568026229</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11">
         <v>4097951028</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11">
         <v>8066789201</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11">
         <v>2144253105</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11">
         <v>2147188294</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="G14" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11">
         <v>2109989692</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="G15" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11">
         <v>2067957492</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11">
         <v>5126355765</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="G17" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11">
         <v>2107925272</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="G18" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11">
         <v>8328363654</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="G19" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11">
         <v>3619468307</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="G20" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11">
         <v>2815434485</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="G21" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11">
         <v>9729750941</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="C22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="G22" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11">
         <v>9366155632</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="12" t="s">
+      <c r="C23" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="G23" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11">
         <v>5127740651</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="G24" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11">
         <v>2107764291</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="G25" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11">
         <v>5126889568</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="G26" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11">
         <v>2144762616</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="12" t="s">
+      <c r="C27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="G27" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11">
         <v>4614611617</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="12" t="s">
+      <c r="C28" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="G28" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11">
         <v>3619456914</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="C29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="G29" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11">
         <v>2108457189</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="12" t="s">
+      <c r="C30" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="G30" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11">
         <v>8326847483</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="12" t="s">
+      <c r="C31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="G31" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11">
         <v>5128105776</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="12" t="s">
+      <c r="C32" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="G32" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11">
         <v>2149956490</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="12" t="s">
+      <c r="C33" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="G33" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11">
         <v>8323595785</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="G34" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11">
         <v>3616589810</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="12" t="s">
+      <c r="C35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="G35" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11">
         <v>5129975898</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="G36" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11">
         <v>4694752375</v>
       </c>
-      <c r="C37" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="12" t="s">
+      <c r="C37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="G37" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11">
         <v>4696171489</v>
       </c>
-      <c r="C38" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="12" t="s">
+      <c r="C38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="G38" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11">
         <v>8308220360</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="G39" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11">
         <v>8328083248</v>
       </c>
-      <c r="C40" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="12" t="s">
+      <c r="C40" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="G40" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11">
         <v>9366486460</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="12" t="s">
+      <c r="C41" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="G41" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11">
         <v>8302370080</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="G42" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11">
         <v>2253337271</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="12" t="s">
+      <c r="C43" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="G43" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11">
         <v>4698317311</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="12" t="s">
+      <c r="C44" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="G44" s="11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11">
         <v>9568324204</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="12" t="s">
+      <c r="C45" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="G45" s="11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B46" s="9"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B47" s="9"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B48" s="9"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="9"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B50" s="9"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="9"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B52" s="9"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53" s="9"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B54" s="9"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B55" s="9"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B56" s="9"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B57" s="9"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B58" s="9"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B59" s="9"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B60" s="9"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="8"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" s="8"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" s="8"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" s="8"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" s="8"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" s="8"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" s="8"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" s="8"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" s="8"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" s="8"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56" s="8"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" s="8"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58" s="8"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59" s="8"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60" s="8"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" sort="0"/>

</xml_diff>